<commit_message>
add compiler optimization comparison
</commit_message>
<xml_diff>
--- a/評価.xlsx
+++ b/評価.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3C6762-BD6E-4C65-AC15-FBD11215A5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2A2BF8-9D40-4768-B5D7-7657C667379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="処理時間(machineA)" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>avg</t>
   </si>
@@ -114,6 +114,38 @@
   </si>
   <si>
     <t>逐次</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>なし</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>あり</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>最適化(O2)</t>
+    <rPh sb="0" eb="3">
+      <t>サイテキカ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>逐次</t>
+  </si>
+  <si>
+    <t>最適化O2なし</t>
+    <rPh sb="0" eb="3">
+      <t>サイテキカ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>最適化O2あり</t>
+    <rPh sb="0" eb="3">
+      <t>サイテキカ</t>
+    </rPh>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -739,7 +771,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,6 +790,12 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,9 +803,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -876,23 +911,27 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
               <a:t>処理速度</a:t>
             </a:r>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>(machine A)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -909,16 +948,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ja-JP"/>
@@ -929,17 +968,26 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'処理時間(machineA)'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>最適化O2あり</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -947,67 +995,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.000_);[Red]\(#,##0.000\)" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'処理時間(machineA)'!$B$1:$E$1</c:f>
+              <c:f>'処理時間(machineA)'!$L$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1028,7 +1018,79 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'処理時間(machineA)'!$B$12:$E$12</c:f>
+              <c:f>'処理時間(machineA)'!$L$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.6082280000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6232099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1733348000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49824000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E3E-4CBA-AFFB-7B352A9E3A41}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'処理時間(machineA)'!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>最適化O2なし</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'処理時間(machineA)'!$L$1:$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐次</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OpenMP
+(parallel for)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVX2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OpenMP+AVX2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'処理時間(machineA)'!$L$2:$O$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1042,38 +1104,102 @@
                   <c:v>3.5178693999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0950095999999998</c:v>
+                  <c:v>1.0950096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-61B1-4E11-8DF0-AF5AF72B23C6}"/>
+              <c16:uniqueId val="{00000000-3E3E-4CBA-AFFB-7B352A9E3A41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="80"/>
-        <c:overlap val="25"/>
-        <c:axId val="1234603199"/>
-        <c:axId val="1234600287"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="393471184"/>
+        <c:axId val="393477424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1234603199"/>
+        <c:axId val="393471184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393477424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="393477424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="18"/>
+        </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1081,7 +1207,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1094,9 +1220,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>処理方法</a:t>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>時間</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>秒</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1113,7 +1252,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1130,19 +1269,13 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1151,7 +1284,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1166,134 +1299,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1234600287"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1234600287"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>時間</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>(</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>秒</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>)</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1234603199"/>
+        <c:crossAx val="393471184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1305,13 +1311,44 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -1363,23 +1400,27 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
               <a:t>処理速度</a:t>
             </a:r>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>(machine B)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1396,16 +1437,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ja-JP"/>
@@ -1416,17 +1457,26 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'処理時間(machineB)'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>最適化O2あり</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1434,67 +1484,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.000_);[Red]\(#,##0.000\)" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'処理時間(machineB)'!$B$1:$E$1</c:f>
+              <c:f>'処理時間(machineB)'!$L$1:$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1515,7 +1507,79 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'処理時間(machineB)'!$B$12:$E$12</c:f>
+              <c:f>'処理時間(machineB)'!$L$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.9083847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8771526000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4218424999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3548708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB84-4AFE-B20C-09135B348DDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'処理時間(machineB)'!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>最適化O2なし</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'処理時間(machineB)'!$L$1:$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>逐次</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OpenMP
+(parallel for)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVX2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OpenMP+AVX2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'処理時間(machineB)'!$L$2:$O$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1529,38 +1593,101 @@
                   <c:v>5.835064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5532732000000005</c:v>
+                  <c:v>2.5532732</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-056D-4B1F-A1F0-3816D1658FA8}"/>
+              <c16:uniqueId val="{00000001-EB84-4AFE-B20C-09135B348DDC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="80"/>
-        <c:overlap val="25"/>
-        <c:axId val="1234603199"/>
-        <c:axId val="1234600287"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="393471184"/>
+        <c:axId val="393477424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1234603199"/>
+        <c:axId val="393471184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393477424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="393477424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1568,7 +1695,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1581,9 +1708,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>処理方法</a:t>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>時間</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>秒</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1600,7 +1740,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1617,19 +1757,13 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1638,7 +1772,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1653,134 +1787,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1234600287"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1234600287"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>時間</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>(</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="ja-JP"/>
-                  <a:t>秒</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>)</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1234603199"/>
+        <c:crossAx val="393471184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1792,13 +1799,44 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2351,990 +2389,6 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="bg1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="bg1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3839,33 +2893,1041 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>578827</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>319088</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219809</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>89388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="グラフ 3">
+        <xdr:cNvPr id="2" name="グラフ 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96FE8559-7DBF-4478-8AFB-C4EBBA5352BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC004538-1C20-4CB9-A7AC-8F4D15915E7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3886,27 +3948,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>633411</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>109172</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1">
+        <xdr:cNvPr id="3" name="グラフ 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{075DDDCB-2025-47FC-BD39-87250A57212D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{983BDE5C-A1E6-42E0-83F7-79DC10E28256}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4341,223 +4405,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960D7322-F6C4-4493-9AE0-2462C084FC23}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>11.7276974</v>
+      </c>
+      <c r="M2">
+        <v>3.5271202000000001</v>
+      </c>
+      <c r="N2">
+        <v>3.5178693999999999</v>
+      </c>
+      <c r="O2">
+        <v>1.0950096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>4.6082280000000004</v>
+      </c>
+      <c r="M3">
+        <v>1.6232099</v>
+      </c>
+      <c r="N3">
+        <v>2.1733348000000001</v>
+      </c>
+      <c r="O3">
+        <v>0.49824000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>11.898199999999999</v>
+      </c>
+      <c r="C4">
+        <v>4.2526609999999998</v>
+      </c>
+      <c r="D4">
+        <v>3.0342440000000002</v>
+      </c>
+      <c r="E4">
+        <v>1.5487150000000001</v>
+      </c>
+      <c r="F4">
+        <v>3.450488</v>
+      </c>
+      <c r="G4">
+        <v>2.1387360000000002</v>
+      </c>
+      <c r="H4">
+        <v>0.98907900000000004</v>
+      </c>
+      <c r="I4">
+        <v>0.48886600000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>11.142144999999999</v>
+      </c>
+      <c r="C5">
+        <v>4.2642870000000004</v>
+      </c>
+      <c r="D5">
+        <v>3.198213</v>
+      </c>
+      <c r="E5">
+        <v>1.5214939999999999</v>
+      </c>
+      <c r="F5">
+        <v>3.1990569999999998</v>
+      </c>
+      <c r="G5">
+        <v>1.9887090000000001</v>
+      </c>
+      <c r="H5">
+        <v>1.0288740000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.48433300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
+      <c r="B6">
+        <v>11.127146</v>
+      </c>
+      <c r="C6">
+        <v>4.260834</v>
+      </c>
+      <c r="D6">
+        <v>3.33968</v>
+      </c>
+      <c r="E6">
+        <v>1.6636679999999999</v>
+      </c>
+      <c r="F6">
+        <v>3.3128410000000001</v>
+      </c>
+      <c r="G6">
+        <v>2.1922229999999998</v>
+      </c>
+      <c r="H6">
+        <v>1.0610120000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.51637</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>11.898199999999999</v>
-      </c>
-      <c r="C2">
-        <v>3.0342440000000002</v>
-      </c>
-      <c r="D2">
-        <v>3.450488</v>
-      </c>
-      <c r="E2">
-        <v>0.98907900000000004</v>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>11.404442</v>
+      </c>
+      <c r="C7">
+        <v>4.6622979999999998</v>
+      </c>
+      <c r="D7">
+        <v>3.5353300000000001</v>
+      </c>
+      <c r="E7">
+        <v>1.6665049999999999</v>
+      </c>
+      <c r="F7">
+        <v>3.2906490000000002</v>
+      </c>
+      <c r="G7">
+        <v>2.2325729999999999</v>
+      </c>
+      <c r="H7">
+        <v>1.1148830000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.48500500000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>11.142144999999999</v>
-      </c>
-      <c r="C3">
-        <v>3.198213</v>
-      </c>
-      <c r="D3">
-        <v>3.1990569999999998</v>
-      </c>
-      <c r="E3">
-        <v>1.0288740000000001</v>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>11.842518</v>
+      </c>
+      <c r="C8">
+        <v>4.7366650000000003</v>
+      </c>
+      <c r="D8">
+        <v>3.583615</v>
+      </c>
+      <c r="E8">
+        <v>1.5753539999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.306508</v>
+      </c>
+      <c r="G8">
+        <v>2.103418</v>
+      </c>
+      <c r="H8">
+        <v>1.083688</v>
+      </c>
+      <c r="I8">
+        <v>0.49250500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>11.127146</v>
-      </c>
-      <c r="C4">
-        <v>3.33968</v>
-      </c>
-      <c r="D4">
-        <v>3.3128410000000001</v>
-      </c>
-      <c r="E4">
-        <v>1.0610120000000001</v>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>11.319900000000001</v>
+      </c>
+      <c r="C9">
+        <v>4.6245989999999999</v>
+      </c>
+      <c r="D9">
+        <v>3.6056819999999998</v>
+      </c>
+      <c r="E9">
+        <v>1.626109</v>
+      </c>
+      <c r="F9">
+        <v>3.7244250000000001</v>
+      </c>
+      <c r="G9">
+        <v>2.2590949999999999</v>
+      </c>
+      <c r="H9">
+        <v>1.1624410000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.48344100000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>11.404442</v>
-      </c>
-      <c r="C5">
-        <v>3.5353300000000001</v>
-      </c>
-      <c r="D5">
-        <v>3.2906490000000002</v>
-      </c>
-      <c r="E5">
-        <v>1.1148830000000001</v>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>11.816893</v>
+      </c>
+      <c r="C10">
+        <v>4.4075139999999999</v>
+      </c>
+      <c r="D10">
+        <v>3.6952609999999999</v>
+      </c>
+      <c r="E10">
+        <v>1.716466</v>
+      </c>
+      <c r="F10">
+        <v>3.4089770000000001</v>
+      </c>
+      <c r="G10">
+        <v>2.2153179999999999</v>
+      </c>
+      <c r="H10">
+        <v>1.120938</v>
+      </c>
+      <c r="I10">
+        <v>0.48324400000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>11.842518</v>
-      </c>
-      <c r="C6">
-        <v>3.583615</v>
-      </c>
-      <c r="D6">
-        <v>3.306508</v>
-      </c>
-      <c r="E6">
-        <v>1.083688</v>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>12.138064</v>
+      </c>
+      <c r="C11">
+        <v>4.8022010000000002</v>
+      </c>
+      <c r="D11">
+        <v>3.7663639999999998</v>
+      </c>
+      <c r="E11">
+        <v>1.6334960000000001</v>
+      </c>
+      <c r="F11">
+        <v>3.422701</v>
+      </c>
+      <c r="G11">
+        <v>2.130779</v>
+      </c>
+      <c r="H11">
+        <v>1.1427929999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.52501399999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>11.319900000000001</v>
-      </c>
-      <c r="C7">
-        <v>3.6056819999999998</v>
-      </c>
-      <c r="D7">
-        <v>3.7244250000000001</v>
-      </c>
-      <c r="E7">
-        <v>1.1624410000000001</v>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>11.886473000000001</v>
+      </c>
+      <c r="C12">
+        <v>5.0490709999999996</v>
+      </c>
+      <c r="D12">
+        <v>3.7541769999999999</v>
+      </c>
+      <c r="E12">
+        <v>1.6702710000000001</v>
+      </c>
+      <c r="F12">
+        <v>4.3699859999999999</v>
+      </c>
+      <c r="G12">
+        <v>2.2499880000000001</v>
+      </c>
+      <c r="H12">
+        <v>1.106125</v>
+      </c>
+      <c r="I12">
+        <v>0.47775400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>11.816893</v>
-      </c>
-      <c r="C8">
-        <v>3.6952609999999999</v>
-      </c>
-      <c r="D8">
-        <v>3.4089770000000001</v>
-      </c>
-      <c r="E8">
-        <v>1.120938</v>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>12.701193</v>
+      </c>
+      <c r="C13">
+        <v>5.0221499999999999</v>
+      </c>
+      <c r="D13">
+        <v>3.7586360000000001</v>
+      </c>
+      <c r="E13">
+        <v>1.6100209999999999</v>
+      </c>
+      <c r="F13">
+        <v>3.6930619999999998</v>
+      </c>
+      <c r="G13">
+        <v>2.2225090000000001</v>
+      </c>
+      <c r="H13">
+        <v>1.140263</v>
+      </c>
+      <c r="I13">
+        <v>0.54586800000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>12.138064</v>
-      </c>
-      <c r="C9">
-        <v>3.7663639999999998</v>
-      </c>
-      <c r="D9">
-        <v>3.422701</v>
-      </c>
-      <c r="E9">
-        <v>1.1427929999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>11.886473000000001</v>
-      </c>
-      <c r="C10">
-        <v>3.7541769999999999</v>
-      </c>
-      <c r="D10">
-        <v>4.3699859999999999</v>
-      </c>
-      <c r="E10">
-        <v>1.106125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>12.701193</v>
-      </c>
-      <c r="C11">
-        <v>3.7586360000000001</v>
-      </c>
-      <c r="D11">
-        <v>3.6930619999999998</v>
-      </c>
-      <c r="E11">
-        <v>1.140263</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
-        <f>AVERAGE(B2:B11)</f>
+      <c r="B14" s="1">
+        <f t="shared" ref="B14:I14" si="0">AVERAGE(B4:B13)</f>
         <v>11.7276974</v>
       </c>
-      <c r="C12" s="1">
-        <f>AVERAGE(C2:C11)</f>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6082279999999995</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
         <v>3.5271202000000001</v>
       </c>
-      <c r="D12" s="1">
-        <f>AVERAGE(D2:D11)</f>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6232098999999998</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
         <v>3.5178693999999999</v>
       </c>
-      <c r="E12" s="1">
-        <f>AVERAGE(E2:E11)</f>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1733347999999997</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
         <v>1.0950095999999998</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49824000000000002</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4567,223 +4851,442 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>16.012982099999999</v>
+      </c>
+      <c r="M2">
+        <v>8.5621843000000002</v>
+      </c>
+      <c r="N2">
+        <v>5.835064</v>
+      </c>
+      <c r="O2">
+        <v>2.5532732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>3.9083847</v>
+      </c>
+      <c r="M3">
+        <v>1.8771526000000001</v>
+      </c>
+      <c r="N3">
+        <v>3.4218424999999999</v>
+      </c>
+      <c r="O3">
+        <v>1.3548708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>15.962113</v>
+      </c>
+      <c r="C4">
+        <v>4.0954259999999998</v>
+      </c>
+      <c r="D4">
+        <v>8.7998220000000007</v>
+      </c>
+      <c r="E4">
+        <v>1.8589979999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.7655419999999999</v>
+      </c>
+      <c r="G4">
+        <v>3.30722</v>
+      </c>
+      <c r="H4">
+        <v>2.5619990000000001</v>
+      </c>
+      <c r="I4">
+        <v>1.2672190000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>15.978859</v>
+      </c>
+      <c r="C5">
+        <v>4.0601320000000003</v>
+      </c>
+      <c r="D5">
+        <v>8.8862360000000002</v>
+      </c>
+      <c r="E5">
+        <v>1.877232</v>
+      </c>
+      <c r="F5">
+        <v>5.8336249999999996</v>
+      </c>
+      <c r="G5">
+        <v>3.2800699999999998</v>
+      </c>
+      <c r="H5">
+        <v>2.5511659999999998</v>
+      </c>
+      <c r="I5">
+        <v>1.262699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B6">
+        <v>15.960027999999999</v>
+      </c>
+      <c r="C6">
+        <v>4.0721790000000002</v>
+      </c>
+      <c r="D6">
+        <v>8.7614959999999993</v>
+      </c>
+      <c r="E6">
+        <v>1.873219</v>
+      </c>
+      <c r="F6">
+        <v>5.8447139999999997</v>
+      </c>
+      <c r="G6">
+        <v>3.2882560000000001</v>
+      </c>
+      <c r="H6">
+        <v>2.5601759999999998</v>
+      </c>
+      <c r="I6">
+        <v>1.496731</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>16.050352</v>
+      </c>
+      <c r="C7">
+        <v>3.735144</v>
+      </c>
+      <c r="D7">
+        <v>8.7669610000000002</v>
+      </c>
+      <c r="E7">
+        <v>1.882053</v>
+      </c>
+      <c r="F7">
+        <v>5.7947150000000001</v>
+      </c>
+      <c r="G7">
+        <v>3.3014809999999999</v>
+      </c>
+      <c r="H7">
+        <v>2.5835669999999999</v>
+      </c>
+      <c r="I7">
+        <v>1.446566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>15.961954</v>
+      </c>
+      <c r="C8">
+        <v>3.7537959999999999</v>
+      </c>
+      <c r="D8">
+        <v>8.7728300000000008</v>
+      </c>
+      <c r="E8">
+        <v>1.857081</v>
+      </c>
+      <c r="F8">
+        <v>5.8800949999999998</v>
+      </c>
+      <c r="G8">
+        <v>3.3231039999999998</v>
+      </c>
+      <c r="H8">
+        <v>2.4975610000000001</v>
+      </c>
+      <c r="I8">
+        <v>1.4456150000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>16.013639000000001</v>
+      </c>
+      <c r="C9">
+        <v>3.741107</v>
+      </c>
+      <c r="D9">
+        <v>8.9230359999999997</v>
+      </c>
+      <c r="E9">
+        <v>1.866916</v>
+      </c>
+      <c r="F9">
+        <v>5.9415440000000004</v>
+      </c>
+      <c r="G9">
+        <v>3.3512390000000001</v>
+      </c>
+      <c r="H9">
+        <v>2.5574699999999999</v>
+      </c>
+      <c r="I9">
+        <v>1.2479039999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>15.951714000000001</v>
+      </c>
+      <c r="C10">
+        <v>4.0676329999999998</v>
+      </c>
+      <c r="D10">
+        <v>6.1525910000000001</v>
+      </c>
+      <c r="E10">
+        <v>1.8996569999999999</v>
+      </c>
+      <c r="F10">
+        <v>5.8627159999999998</v>
+      </c>
+      <c r="G10">
+        <v>3.3445809999999998</v>
+      </c>
+      <c r="H10">
+        <v>2.5378579999999999</v>
+      </c>
+      <c r="I10">
+        <v>1.402577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>15.961563999999999</v>
+      </c>
+      <c r="C11">
+        <v>3.9047839999999998</v>
+      </c>
+      <c r="D11">
+        <v>8.8750420000000005</v>
+      </c>
+      <c r="E11">
+        <v>1.8929609999999999</v>
+      </c>
+      <c r="F11">
+        <v>5.8520019999999997</v>
+      </c>
+      <c r="G11">
+        <v>3.3521359999999998</v>
+      </c>
+      <c r="H11">
+        <v>2.5855860000000002</v>
+      </c>
+      <c r="I11">
+        <v>1.459244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>15.965767</v>
+      </c>
+      <c r="C12">
+        <v>3.9656400000000001</v>
+      </c>
+      <c r="D12">
+        <v>8.8856739999999999</v>
+      </c>
+      <c r="E12">
+        <v>1.898871</v>
+      </c>
+      <c r="F12">
+        <v>5.8226750000000003</v>
+      </c>
+      <c r="G12">
+        <v>3.8341090000000002</v>
+      </c>
+      <c r="H12">
+        <v>2.5353490000000001</v>
+      </c>
+      <c r="I12">
+        <v>1.3016810000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
+      <c r="B13">
+        <v>16.323830999999998</v>
+      </c>
+      <c r="C13">
+        <v>3.6880060000000001</v>
+      </c>
+      <c r="D13">
+        <v>8.7981549999999995</v>
+      </c>
+      <c r="E13">
+        <v>1.864538</v>
+      </c>
+      <c r="F13">
+        <v>5.753012</v>
+      </c>
+      <c r="G13">
+        <v>3.8362289999999999</v>
+      </c>
+      <c r="H13">
+        <v>2.5619999999999998</v>
+      </c>
+      <c r="I13">
+        <v>1.218472</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>15.962113</v>
-      </c>
-      <c r="C2">
-        <v>8.7998220000000007</v>
-      </c>
-      <c r="D2">
-        <v>5.7655419999999999</v>
-      </c>
-      <c r="E2">
-        <v>2.5619990000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>15.978859</v>
-      </c>
-      <c r="C3">
-        <v>8.8862360000000002</v>
-      </c>
-      <c r="D3">
-        <v>5.8336249999999996</v>
-      </c>
-      <c r="E3">
-        <v>2.5511659999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>15.960027999999999</v>
-      </c>
-      <c r="C4">
-        <v>8.7614959999999993</v>
-      </c>
-      <c r="D4">
-        <v>5.8447139999999997</v>
-      </c>
-      <c r="E4">
-        <v>2.5601759999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>16.050352</v>
-      </c>
-      <c r="C5">
-        <v>8.7669610000000002</v>
-      </c>
-      <c r="D5">
-        <v>5.7947150000000001</v>
-      </c>
-      <c r="E5">
-        <v>2.5835669999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>15.961954</v>
-      </c>
-      <c r="C6">
-        <v>8.7728300000000008</v>
-      </c>
-      <c r="D6">
-        <v>5.8800949999999998</v>
-      </c>
-      <c r="E6">
-        <v>2.4975610000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>16.013639000000001</v>
-      </c>
-      <c r="C7">
-        <v>8.9230359999999997</v>
-      </c>
-      <c r="D7">
-        <v>5.9415440000000004</v>
-      </c>
-      <c r="E7">
-        <v>2.5574699999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>15.951714000000001</v>
-      </c>
-      <c r="C8">
-        <v>6.1525910000000001</v>
-      </c>
-      <c r="D8">
-        <v>5.8627159999999998</v>
-      </c>
-      <c r="E8">
-        <v>2.5378579999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>15.961563999999999</v>
-      </c>
-      <c r="C9">
-        <v>8.8750420000000005</v>
-      </c>
-      <c r="D9">
-        <v>5.8520019999999997</v>
-      </c>
-      <c r="E9">
-        <v>2.5855860000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>15.965767</v>
-      </c>
-      <c r="C10">
-        <v>8.8856739999999999</v>
-      </c>
-      <c r="D10">
-        <v>5.8226750000000003</v>
-      </c>
-      <c r="E10">
-        <v>2.5353490000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>16.323830999999998</v>
-      </c>
-      <c r="C11">
-        <v>8.7981549999999995</v>
-      </c>
-      <c r="D11">
-        <v>5.753012</v>
-      </c>
-      <c r="E11">
-        <v>2.5619999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
-        <f>AVERAGE(B2:B11)</f>
+      <c r="B14" s="1">
+        <f t="shared" ref="B14:I14" si="0">AVERAGE(B4:B13)</f>
         <v>16.012982099999999</v>
       </c>
-      <c r="C12" s="1">
-        <f>AVERAGE(C2:C11)</f>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9083847</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
         <v>8.5621843000000002</v>
       </c>
-      <c r="D12" s="1">
-        <f>AVERAGE(D2:D11)</f>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8771525999999998</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
         <v>5.835064</v>
       </c>
-      <c r="E12" s="1">
-        <f>AVERAGE(E2:E11)</f>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4218425000000003</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
         <v>2.5532732000000005</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3548708</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4795,8 +5298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D40129C-2561-4ACA-AD82-CCA0D4DE21D7}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4821,26 +5324,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="33" x14ac:dyDescent="0.4">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="T1" s="6" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="T1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">

</xml_diff>